<commit_message>
Enable hydrogen flow to all the sectors
</commit_message>
<xml_diff>
--- a/VT_IE_AGR.xlsx
+++ b/VT_IE_AGR.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F73DD7BD-A07A-4AB7-849E-6BA3A0320430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451E2168-3A4A-4720-8F2D-8F2470B3CC09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="31" r:id="rId1"/>
@@ -3803,12 +3803,6 @@
     <t>AGRHET</t>
   </si>
   <si>
-    <t>SUPH2GD</t>
-  </si>
-  <si>
-    <t>SUPH2LD</t>
-  </si>
-  <si>
     <t>Output~2012</t>
   </si>
   <si>
@@ -4098,6 +4092,12 @@
   </si>
   <si>
     <t>~FI_T: MEUR2000</t>
+  </si>
+  <si>
+    <t>H2GMD, H2GHD</t>
+  </si>
+  <si>
+    <t>H2LD</t>
   </si>
 </sst>
 </file>
@@ -5795,6 +5795,12 @@
     <xf numFmtId="0" fontId="38" fillId="19" borderId="0" xfId="5" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="19" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -5806,12 +5812,6 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -19580,9 +19580,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -19620,9 +19620,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -19655,26 +19655,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -19707,26 +19690,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -20342,12 +20308,12 @@
       <c r="Z15" s="322"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="338" t="s">
-        <v>684</v>
-      </c>
-      <c r="B16" s="338"/>
-      <c r="C16" s="338"/>
-      <c r="D16" s="338"/>
+      <c r="A16" s="340" t="s">
+        <v>682</v>
+      </c>
+      <c r="B16" s="340"/>
+      <c r="C16" s="340"/>
+      <c r="D16" s="340"/>
       <c r="E16" s="324"/>
       <c r="F16" s="324"/>
       <c r="G16" s="325"/>
@@ -20429,13 +20395,13 @@
     </row>
     <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="329" t="s">
-        <v>685</v>
-      </c>
-      <c r="B19" s="337" t="s">
-        <v>696</v>
-      </c>
-      <c r="C19" s="337"/>
-      <c r="D19" s="337"/>
+        <v>683</v>
+      </c>
+      <c r="B19" s="339" t="s">
+        <v>694</v>
+      </c>
+      <c r="C19" s="339"/>
+      <c r="D19" s="339"/>
       <c r="E19" s="330"/>
       <c r="F19" s="330"/>
       <c r="G19" s="331"/>
@@ -20461,13 +20427,13 @@
     </row>
     <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="329" t="s">
-        <v>686</v>
-      </c>
-      <c r="B20" s="337" t="s">
-        <v>697</v>
-      </c>
-      <c r="C20" s="337"/>
-      <c r="D20" s="337"/>
+        <v>684</v>
+      </c>
+      <c r="B20" s="339" t="s">
+        <v>695</v>
+      </c>
+      <c r="C20" s="339"/>
+      <c r="D20" s="339"/>
       <c r="E20" s="330"/>
       <c r="F20" s="330"/>
       <c r="G20" s="331"/>
@@ -20493,10 +20459,10 @@
     </row>
     <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="329" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="B21" s="332" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="C21" s="332"/>
       <c r="D21" s="332"/>
@@ -20553,13 +20519,13 @@
     </row>
     <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="329" t="s">
-        <v>688</v>
-      </c>
-      <c r="B23" s="337" t="s">
-        <v>699</v>
-      </c>
-      <c r="C23" s="337"/>
-      <c r="D23" s="337"/>
+        <v>686</v>
+      </c>
+      <c r="B23" s="339" t="s">
+        <v>697</v>
+      </c>
+      <c r="C23" s="339"/>
+      <c r="D23" s="339"/>
       <c r="E23" s="322"/>
       <c r="F23" s="322"/>
       <c r="G23" s="322"/>
@@ -20641,13 +20607,13 @@
     </row>
     <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="329" t="s">
-        <v>689</v>
-      </c>
-      <c r="B26" s="337" t="s">
-        <v>700</v>
-      </c>
-      <c r="C26" s="337"/>
-      <c r="D26" s="337"/>
+        <v>687</v>
+      </c>
+      <c r="B26" s="339" t="s">
+        <v>698</v>
+      </c>
+      <c r="C26" s="339"/>
+      <c r="D26" s="339"/>
       <c r="E26" s="322"/>
       <c r="F26" s="322"/>
       <c r="G26" s="322"/>
@@ -20729,7 +20695,7 @@
     </row>
     <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="329" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B29" s="333">
         <v>1</v>
@@ -20761,13 +20727,13 @@
     </row>
     <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="329" t="s">
-        <v>691</v>
-      </c>
-      <c r="B30" s="339" t="s">
-        <v>692</v>
-      </c>
-      <c r="C30" s="337"/>
-      <c r="D30" s="337"/>
+        <v>689</v>
+      </c>
+      <c r="B30" s="341" t="s">
+        <v>690</v>
+      </c>
+      <c r="C30" s="339"/>
+      <c r="D30" s="339"/>
       <c r="E30" s="334"/>
       <c r="F30" s="334"/>
       <c r="G30" s="322"/>
@@ -20793,13 +20759,13 @@
     </row>
     <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="329" t="s">
-        <v>693</v>
-      </c>
-      <c r="B31" s="337" t="s">
-        <v>694</v>
-      </c>
-      <c r="C31" s="337"/>
-      <c r="D31" s="337"/>
+        <v>691</v>
+      </c>
+      <c r="B31" s="339" t="s">
+        <v>692</v>
+      </c>
+      <c r="C31" s="339"/>
+      <c r="D31" s="339"/>
       <c r="E31" s="334"/>
       <c r="F31" s="334"/>
       <c r="G31" s="322"/>
@@ -20826,7 +20792,7 @@
     <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="335"/>
       <c r="B32" s="336" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="C32" s="335"/>
       <c r="D32" s="335"/>
@@ -22780,13 +22746,13 @@
   <sheetData>
     <row r="3" spans="2:34" x14ac:dyDescent="0.2">
       <c r="F3" s="3" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="2:34" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B4" s="243" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="C4" s="243" t="s">
         <v>1</v>
@@ -22866,7 +22832,7 @@
     </row>
     <row r="5" spans="2:34" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="24" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="C5" s="24" t="s">
         <v>31</v>
@@ -25515,12 +25481,12 @@
     <row r="1" spans="2:20" ht="6.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:20" x14ac:dyDescent="0.2">
       <c r="F2" s="3" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
     </row>
     <row r="3" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B3" s="23" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="C3" s="23" t="s">
         <v>1</v>
@@ -25568,10 +25534,10 @@
         <v>292</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="T3" s="4" t="s">
         <v>293</v>
@@ -25579,7 +25545,7 @@
     </row>
     <row r="4" spans="2:20" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="24" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="C4" s="24" t="s">
         <v>31</v>
@@ -25611,7 +25577,7 @@
         <v>37</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="S4" s="5" t="s">
         <v>37</v>
@@ -30342,24 +30308,24 @@
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B3" s="242" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" s="243" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="341" t="str">
+      <c r="C4" s="337" t="str">
         <f>Regions!C3</f>
         <v>IE</v>
       </c>
-      <c r="D4" s="341" t="str">
+      <c r="D4" s="337" t="str">
         <f>Regions!D3</f>
         <v>National</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="342" t="s">
+      <c r="B5" s="338" t="s">
         <v>153</v>
       </c>
       <c r="C5" s="244"/>
@@ -30586,10 +30552,10 @@
       <c r="E1" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="340" t="s">
+      <c r="F1" s="342" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="340" t="s">
+      <c r="G1" s="342" t="s">
         <v>12</v>
       </c>
       <c r="H1" s="27" t="s">
@@ -30670,8 +30636,8 @@
       <c r="C2" s="25"/>
       <c r="D2" s="26"/>
       <c r="E2" s="26"/>
-      <c r="F2" s="340"/>
-      <c r="G2" s="340"/>
+      <c r="F2" s="342"/>
+      <c r="G2" s="342"/>
       <c r="H2" s="149" t="s">
         <v>570</v>
       </c>
@@ -37945,28 +37911,28 @@
       <c r="E1" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="340" t="s">
+      <c r="F1" s="342" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="340" t="s">
+      <c r="G1" s="342" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="340" t="s">
+      <c r="H1" s="342" t="s">
         <v>591</v>
       </c>
-      <c r="I1" s="340" t="s">
+      <c r="I1" s="342" t="s">
         <v>592</v>
       </c>
-      <c r="J1" s="340" t="s">
+      <c r="J1" s="342" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="340" t="s">
+      <c r="K1" s="342" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="340" t="s">
+      <c r="L1" s="342" t="s">
         <v>430</v>
       </c>
-      <c r="M1" s="340" t="s">
+      <c r="M1" s="342" t="s">
         <v>431</v>
       </c>
       <c r="N1" s="27" t="s">
@@ -38028,14 +37994,14 @@
       <c r="C2" s="25"/>
       <c r="D2" s="26"/>
       <c r="E2" s="26"/>
-      <c r="F2" s="340"/>
-      <c r="G2" s="340"/>
-      <c r="H2" s="340"/>
-      <c r="I2" s="340"/>
-      <c r="J2" s="340"/>
-      <c r="K2" s="340"/>
-      <c r="L2" s="340"/>
-      <c r="M2" s="340"/>
+      <c r="F2" s="342"/>
+      <c r="G2" s="342"/>
+      <c r="H2" s="342"/>
+      <c r="I2" s="342"/>
+      <c r="J2" s="342"/>
+      <c r="K2" s="342"/>
+      <c r="L2" s="342"/>
+      <c r="M2" s="342"/>
       <c r="N2" s="149" t="s">
         <v>570</v>
       </c>
@@ -53660,13 +53626,13 @@
     </row>
     <row r="5" spans="1:30" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="C5" s="311" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="D5" s="311" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="E5" s="316" t="str">
         <f>A11</f>
@@ -53775,7 +53741,7 @@
     </row>
     <row r="6" spans="1:30" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="C6" s="316" t="str">
         <f>C5</f>
@@ -53892,7 +53858,7 @@
     </row>
     <row r="7" spans="1:30" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="C7" s="316" t="str">
         <f>"*"&amp;C5</f>
@@ -54009,223 +53975,223 @@
     </row>
     <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="312" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="B10" s="312" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" s="313" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="B11" s="313" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12" s="314" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="B12" s="314" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13" s="314" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="B13" s="314" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14" s="314" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="B14" s="314" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15" s="314" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B15" s="314" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16" s="314" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="B16" s="314" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="314" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B17" s="314" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="314" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="B18" s="314" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="314" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="B19" s="314" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="314" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="B20" s="314" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="314" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="B21" s="314" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="314" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B22" s="314" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="314" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="B23" s="314" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="314" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B24" s="314" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="314" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="B25" s="314" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="314" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B26" s="314" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="314" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="B27" s="314" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="314" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B28" s="314" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="314" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="B29" s="314" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="314" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="B30" s="314" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="314" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B31" s="314" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="314" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B32" s="314" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="314" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B33" s="314" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="314" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="B34" s="314" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="314" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="B35" s="314" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="314" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="B36" s="314" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="315" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
     </row>
   </sheetData>
@@ -54304,7 +54270,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="187" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="D4" s="187" t="s">
         <v>1</v>
@@ -56561,8 +56527,8 @@
   </sheetPr>
   <dimension ref="B3:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -56592,7 +56558,7 @@
         <v>118</v>
       </c>
       <c r="C4" s="187" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="D4" s="187" t="s">
         <v>19</v>
@@ -57790,15 +57756,16 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="12.42578125" style="302" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" style="302" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="11.28515625" style="302" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" style="302" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" style="302" customWidth="1"/>
     <col min="6" max="7" width="9.140625" style="302"/>
     <col min="8" max="8" width="10.28515625" style="302" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.5703125" style="302" bestFit="1" customWidth="1"/>
@@ -57838,7 +57805,7 @@
     </row>
     <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="200" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="C4" s="305" t="s">
         <v>1</v>
@@ -57861,7 +57828,7 @@
         <v>4</v>
       </c>
       <c r="L4" s="200" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="M4" s="305" t="s">
         <v>1</v>
@@ -58114,7 +58081,7 @@
         <v>IE,National</v>
       </c>
       <c r="C11" s="302" t="str">
-        <f t="shared" ref="B11:C14" si="0">M8</f>
+        <f t="shared" ref="C11:C14" si="0">M8</f>
         <v>FT-AGRDST</v>
       </c>
       <c r="D11" s="302" t="s">
@@ -58289,11 +58256,11 @@
         <v>IE,National</v>
       </c>
       <c r="C15" s="302" t="str">
-        <f t="shared" ref="B15:C19" si="1">M12</f>
+        <f t="shared" ref="C15:C19" si="1">M12</f>
         <v>FT-AGRHET</v>
       </c>
       <c r="D15" s="319" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="E15" s="302" t="str">
         <f>Commodities!D47</f>
@@ -58404,7 +58371,7 @@
         <v>FT-AGRH2G</v>
       </c>
       <c r="D18" s="310" t="s">
-        <v>609</v>
+        <v>700</v>
       </c>
       <c r="E18" s="302" t="str">
         <f>Commodities!D50</f>
@@ -58427,7 +58394,7 @@
         <v>FT-AGRH2L</v>
       </c>
       <c r="D19" s="310" t="s">
-        <v>610</v>
+        <v>701</v>
       </c>
       <c r="E19" s="302" t="str">
         <f>Commodities!D51</f>
@@ -58521,7 +58488,7 @@
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="200" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="B4" s="200" t="s">
         <v>19</v>
@@ -58688,12 +58655,12 @@
   <sheetData>
     <row r="2" spans="2:31" x14ac:dyDescent="0.2">
       <c r="G2" s="3" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
     </row>
     <row r="3" spans="2:31" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B3" s="243" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="C3" s="243" t="s">
         <v>1</v>
@@ -58750,7 +58717,7 @@
         <v>565</v>
       </c>
       <c r="U3" s="246" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="V3" s="246" t="s">
         <v>182</v>
@@ -58785,7 +58752,7 @@
     </row>
     <row r="4" spans="2:31" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="24" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="C4" s="24" t="s">
         <v>31</v>
@@ -61858,12 +61825,12 @@
   <sheetData>
     <row r="2" spans="2:43" x14ac:dyDescent="0.2">
       <c r="G2" s="3" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
     </row>
     <row r="3" spans="2:43" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B3" s="23" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="C3" s="23" t="s">
         <v>1</v>
@@ -61908,7 +61875,7 @@
         <v>234</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="R3" s="4" t="s">
         <v>182</v>
@@ -61944,7 +61911,7 @@
         <v>17</v>
       </c>
       <c r="AC3" s="4" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="AD3" s="4" t="s">
         <v>362</v>
@@ -61953,16 +61920,16 @@
         <v>363</v>
       </c>
       <c r="AF3" s="4" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="AG3" s="4" t="s">
         <v>364</v>
       </c>
       <c r="AH3" s="4" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="AI3" s="4" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="AJ3" s="4" t="s">
         <v>365</v>
@@ -61974,7 +61941,7 @@
         <v>267</v>
       </c>
       <c r="AM3" s="4" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="AN3" s="4" t="s">
         <v>366</v>
@@ -61988,7 +61955,7 @@
     </row>
     <row r="4" spans="2:43" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="24" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="C4" s="24" t="s">
         <v>31</v>
@@ -66673,12 +66640,12 @@
   <sheetData>
     <row r="2" spans="2:24" x14ac:dyDescent="0.2">
       <c r="G2" s="3" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
     </row>
     <row r="3" spans="2:24" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B3" s="243" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="C3" s="243" t="s">
         <v>1</v>
@@ -66714,7 +66681,7 @@
         <v>565</v>
       </c>
       <c r="N3" s="246" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="O3" s="246" t="s">
         <v>182</v>
@@ -66749,7 +66716,7 @@
     </row>
     <row r="4" spans="2:24" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="24" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="C4" s="24" t="s">
         <v>31</v>

</xml_diff>